<commit_message>
imod-python from .ipynb to Smk
Started preparing the Smk file. Last thing I did was prepare a rule that'll freeze the pixi env if there is anything new. I still have to check it though.
</commit_message>
<xml_diff>
--- a/Mng/Acronyms.xlsx
+++ b/Mng/Acronyms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OD\WS_Mdl\Mng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC01CD98-51AD-493B-8BC9-139F2012DCA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7177CFC-1FA2-41D6-B77D-E863EAE346D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -307,7 +307,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="790">
   <si>
     <t>GW</t>
   </si>
@@ -2666,6 +2666,18 @@
   </si>
   <si>
     <t>GPkg</t>
+  </si>
+  <si>
+    <t>MF6</t>
+  </si>
+  <si>
+    <t>Modflow 6</t>
+  </si>
+  <si>
+    <t>MSW</t>
+  </si>
+  <si>
+    <t>MetaSWAP</t>
   </si>
 </sst>
 </file>
@@ -3204,8 +3216,8 @@
   <dimension ref="A1:F994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C113" sqref="C113"/>
+      <pane ySplit="1" topLeftCell="A353" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C388" sqref="C388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9149,9 +9161,14 @@
       </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B386" s="5"/>
+      <c r="A386" s="5" t="s">
+        <v>786</v>
+      </c>
+      <c r="B386" s="5" t="s">
+        <v>787</v>
+      </c>
       <c r="C386" s="5" t="s">
-        <v>156</v>
+        <v>292</v>
       </c>
       <c r="E386" t="str">
         <f t="shared" si="10"/>
@@ -9159,9 +9176,14 @@
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B387" s="5"/>
+      <c r="A387" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="B387" s="5" t="s">
+        <v>789</v>
+      </c>
       <c r="C387" s="5" t="s">
-        <v>156</v>
+        <v>292</v>
       </c>
       <c r="E387" t="str">
         <f t="shared" si="10"/>

</xml_diff>

<commit_message>
investigating why NBr32 fails to run
NBr32 Sim Ins are written, but some MSW In files are missing and Sim fails to pass MSW results to MF.
I've started investigating why some MSW In files are missing, but I haven't reached a conclussion yet.
Other file-change summary:
setup.py: openpyxl Req added
utils.py: bold print, attempt to run RunMng via pixi (failed)
code/Jupyter/annotate_MSW_In: MSW files annotated
</commit_message>
<xml_diff>
--- a/Mng/Acronyms.xlsx
+++ b/Mng/Acronyms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OD\WS_Mdl\Mng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7177CFC-1FA2-41D6-B77D-E863EAE346D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EB0946-444B-4283-B6A6-14DBED38416B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -307,7 +307,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1810" uniqueCount="792">
   <si>
     <t>GW</t>
   </si>
@@ -2678,6 +2678,12 @@
   </si>
   <si>
     <t>MetaSWAP</t>
+  </si>
+  <si>
+    <t>Py</t>
+  </si>
+  <si>
+    <t>Python</t>
   </si>
 </sst>
 </file>
@@ -3216,8 +3222,8 @@
   <dimension ref="A1:F994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A353" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C388" sqref="C388"/>
+      <pane ySplit="1" topLeftCell="A354" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B389" sqref="B389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9191,9 +9197,14 @@
       </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B388" s="5"/>
+      <c r="A388" s="5" t="s">
+        <v>790</v>
+      </c>
+      <c r="B388" s="5" t="s">
+        <v>791</v>
+      </c>
       <c r="C388" s="5" t="s">
-        <v>156</v>
+        <v>292</v>
       </c>
       <c r="E388" t="str">
         <f t="shared" si="10"/>

</xml_diff>

<commit_message>
functinality to read MSW .inp files
</commit_message>
<xml_diff>
--- a/Mng/Acronyms.xlsx
+++ b/Mng/Acronyms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OD\WS_Mdl\Mng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EB0946-444B-4283-B6A6-14DBED38416B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD61AD9-2CBF-4990-A4C0-502D08D43197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acronyms" sheetId="1" r:id="rId1"/>
@@ -307,7 +307,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1810" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="795">
   <si>
     <t>GW</t>
   </si>
@@ -2684,6 +2684,15 @@
   </si>
   <si>
     <t>Python</t>
+  </si>
+  <si>
+    <t>Auxi</t>
+  </si>
+  <si>
+    <t>Auxilary</t>
+  </si>
+  <si>
+    <t>Not Aux cause it's a windows reserved name, which means you're forbiden for naming folders like this. (Maybe it works in windows, but it definitely doesn't work on OneDrive).</t>
   </si>
 </sst>
 </file>
@@ -9212,9 +9221,17 @@
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B389" s="5"/>
+      <c r="A389" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="B389" s="5" t="s">
+        <v>793</v>
+      </c>
       <c r="C389" s="5" t="s">
-        <v>156</v>
+        <v>300</v>
+      </c>
+      <c r="D389" s="5" t="s">
+        <v>794</v>
       </c>
       <c r="E389" t="str">
         <f t="shared" si="10"/>

</xml_diff>

<commit_message>
SFRmaker #1: Identifying closing erros in WBD SHP
</commit_message>
<xml_diff>
--- a/Mng/Acronyms.xlsx
+++ b/Mng/Acronyms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OD\WS_Mdl\Mng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4421DA8-7193-4A5C-9E39-E7E0D7C21E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4D53C8-367B-408B-9783-E28771FBDE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acronyms" sheetId="1" r:id="rId1"/>
@@ -307,7 +307,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="803">
   <si>
     <t>GW</t>
   </si>
@@ -2699,6 +2699,24 @@
   </si>
   <si>
     <t>Package Data</t>
+  </si>
+  <si>
+    <t>WBD</t>
+  </si>
+  <si>
+    <t>Waterschap Brabantse Delta</t>
+  </si>
+  <si>
+    <t>c_</t>
+  </si>
+  <si>
+    <t>Calculate</t>
+  </si>
+  <si>
+    <t>Dist</t>
+  </si>
+  <si>
+    <t>Distance</t>
   </si>
 </sst>
 </file>
@@ -3237,8 +3255,8 @@
   <dimension ref="A1:F994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A355" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A390" sqref="A390"/>
+      <pane ySplit="1" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B393" sqref="B393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9260,9 +9278,14 @@
       </c>
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B391" s="5"/>
+      <c r="A391" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="B391" t="s">
+        <v>798</v>
+      </c>
       <c r="C391" s="5" t="s">
-        <v>156</v>
+        <v>300</v>
       </c>
       <c r="E391" t="str">
         <f t="shared" si="10"/>
@@ -9270,9 +9293,14 @@
       </c>
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B392" s="5"/>
+      <c r="A392" s="5" t="s">
+        <v>799</v>
+      </c>
+      <c r="B392" s="5" t="s">
+        <v>800</v>
+      </c>
       <c r="C392" s="5" t="s">
-        <v>156</v>
+        <v>292</v>
       </c>
       <c r="E392" t="str">
         <f t="shared" si="10"/>
@@ -9280,9 +9308,14 @@
       </c>
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B393" s="5"/>
+      <c r="A393" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="B393" s="5" t="s">
+        <v>802</v>
+      </c>
       <c r="C393" s="5" t="s">
-        <v>156</v>
+        <v>300</v>
       </c>
       <c r="E393" t="str">
         <f t="shared" si="10"/>

</xml_diff>

<commit_message>
SFRmaker #2: Closing errors identified.
</commit_message>
<xml_diff>
--- a/Mng/Acronyms.xlsx
+++ b/Mng/Acronyms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OD\WS_Mdl\Mng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4D53C8-367B-408B-9783-E28771FBDE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AF5262-CBFF-4ADB-967F-43DF44BC0456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acronyms" sheetId="1" r:id="rId1"/>
@@ -307,7 +307,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="807">
   <si>
     <t>GW</t>
   </si>
@@ -2717,6 +2717,18 @@
   </si>
   <si>
     <t>Distance</t>
+  </si>
+  <si>
+    <t>Prv</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t>Nx</t>
+  </si>
+  <si>
+    <t>Next</t>
   </si>
 </sst>
 </file>
@@ -3256,7 +3268,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B393" sqref="B393"/>
+      <selection pane="bottomLeft" activeCell="C396" sqref="C396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9323,9 +9335,14 @@
       </c>
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B394" s="5"/>
+      <c r="A394" s="5" t="s">
+        <v>803</v>
+      </c>
+      <c r="B394" s="5" t="s">
+        <v>804</v>
+      </c>
       <c r="C394" s="5" t="s">
-        <v>156</v>
+        <v>300</v>
       </c>
       <c r="E394" t="str">
         <f t="shared" si="10"/>
@@ -9333,9 +9350,14 @@
       </c>
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B395" s="5"/>
+      <c r="A395" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="B395" s="5" t="s">
+        <v>806</v>
+      </c>
       <c r="C395" s="5" t="s">
-        <v>156</v>
+        <v>300</v>
       </c>
       <c r="E395" t="str">
         <f t="shared" si="10"/>

</xml_diff>

<commit_message>
SFRmaker #3: loaded .gpkg to Lines
Now we need to connect it to the Sim. Also improved custom character dictionary.
</commit_message>
<xml_diff>
--- a/Mng/Acronyms.xlsx
+++ b/Mng/Acronyms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OD\WS_Mdl\Mng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AF5262-CBFF-4ADB-967F-43DF44BC0456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324D0405-F1F8-4F87-A6EB-38CDEC1BCE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -307,7 +307,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="810">
   <si>
     <t>GW</t>
   </si>
@@ -2122,9 +2122,6 @@
     <t>Elv</t>
   </si>
   <si>
-    <t>Elevation</t>
-  </si>
-  <si>
     <t>Rel</t>
   </si>
   <si>
@@ -2563,9 +2560,6 @@
     <t>UStr</t>
   </si>
   <si>
-    <t>Upsream</t>
-  </si>
-  <si>
     <t>Connection</t>
   </si>
   <si>
@@ -2729,6 +2723,21 @@
   </si>
   <si>
     <t>Next</t>
+  </si>
+  <si>
+    <t>Optl</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>CuCh</t>
+  </si>
+  <si>
+    <t>Custom Character(s)</t>
+  </si>
+  <si>
+    <t>Upsrteam</t>
   </si>
 </sst>
 </file>
@@ -3267,8 +3276,8 @@
   <dimension ref="A1:F994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C396" sqref="C396"/>
+      <pane ySplit="1" topLeftCell="A338" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B354" sqref="B354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3291,7 +3300,7 @@
         <v>155</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>81</v>
@@ -3336,10 +3345,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>424</v>
@@ -3351,10 +3360,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>643</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>644</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>424</v>
@@ -3555,7 +3564,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>58</v>
@@ -3601,16 +3610,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>300</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
@@ -3650,7 +3659,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>51</v>
@@ -3697,10 +3706,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>611</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>612</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>292</v>
@@ -3727,10 +3736,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>292</v>
@@ -3742,10 +3751,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>300</v>
@@ -3773,10 +3782,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>424</v>
@@ -3788,10 +3797,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
+        <v>629</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>630</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>631</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>300</v>
@@ -3879,10 +3888,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>706</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>707</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>300</v>
@@ -3894,10 +3903,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>676</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>677</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>292</v>
@@ -3909,10 +3918,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
+        <v>703</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>704</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>705</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>300</v>
@@ -3939,10 +3948,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>300</v>
@@ -3954,10 +3963,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>745</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>746</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>747</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>300</v>
@@ -3984,10 +3993,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>691</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>692</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>292</v>
@@ -4081,7 +4090,7 @@
         <v>260</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>424</v>
@@ -4108,10 +4117,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>639</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>640</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>300</v>
@@ -4184,10 +4193,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
+        <v>664</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>665</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>666</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>300</v>
@@ -4289,10 +4298,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>292</v>
@@ -4394,10 +4403,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
+        <v>747</v>
+      </c>
+      <c r="B73" s="5" t="s">
         <v>748</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>749</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>292</v>
@@ -4569,7 +4578,7 @@
         <v>603</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>604</v>
+        <v>235</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>292</v>
@@ -4611,10 +4620,10 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="B87" s="5" t="s">
         <v>717</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>718</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>300</v>
@@ -4642,10 +4651,10 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
+        <v>623</v>
+      </c>
+      <c r="B89" s="5" t="s">
         <v>624</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>625</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>300</v>
@@ -4717,10 +4726,10 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
+        <v>640</v>
+      </c>
+      <c r="B94" s="5" t="s">
         <v>641</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>642</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>292</v>
@@ -4838,10 +4847,10 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
+        <v>688</v>
+      </c>
+      <c r="B102" s="5" t="s">
         <v>689</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>690</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>300</v>
@@ -4868,10 +4877,10 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="B104" s="5" t="s">
         <v>710</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>711</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>300</v>
@@ -4883,10 +4892,10 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
+        <v>720</v>
+      </c>
+      <c r="B105" s="5" t="s">
         <v>721</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>722</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>300</v>
@@ -4991,10 +5000,10 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>292</v>
@@ -5131,10 +5140,10 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C121" s="5" t="s">
         <v>300</v>
@@ -5450,10 +5459,10 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="B142" s="5" t="s">
         <v>614</v>
-      </c>
-      <c r="B142" s="5" t="s">
-        <v>615</v>
       </c>
       <c r="C142" s="5" t="s">
         <v>292</v>
@@ -5465,10 +5474,10 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C143" s="5" t="s">
         <v>300</v>
@@ -5510,10 +5519,10 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="B146" s="5" t="s">
         <v>678</v>
-      </c>
-      <c r="B146" s="5" t="s">
-        <v>679</v>
       </c>
       <c r="C146" s="5" t="s">
         <v>300</v>
@@ -5579,7 +5588,7 @@
         <v>424</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E150" t="str">
         <f t="shared" si="4"/>
@@ -5633,10 +5642,10 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="B154" s="5" t="s">
         <v>685</v>
-      </c>
-      <c r="B154" s="5" t="s">
-        <v>686</v>
       </c>
       <c r="C154" s="5" t="s">
         <v>300</v>
@@ -5719,10 +5728,10 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C160" s="5" t="s">
         <v>300</v>
@@ -5734,10 +5743,10 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="B161" s="5" t="s">
         <v>637</v>
-      </c>
-      <c r="B161" s="5" t="s">
-        <v>638</v>
       </c>
       <c r="C161" s="5" t="s">
         <v>292</v>
@@ -5810,7 +5819,7 @@
         <v>296</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E165" t="str">
         <f t="shared" si="5"/>
@@ -5837,7 +5846,7 @@
         <v>294</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C167" s="5" t="s">
         <v>292</v>
@@ -5957,10 +5966,10 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
+        <v>615</v>
+      </c>
+      <c r="B175" s="5" t="s">
         <v>616</v>
-      </c>
-      <c r="B175" s="5" t="s">
-        <v>617</v>
       </c>
       <c r="C175" s="5" t="s">
         <v>292</v>
@@ -6100,13 +6109,13 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="B184" s="5" t="s">
         <v>694</v>
       </c>
-      <c r="B184" s="5" t="s">
+      <c r="C184" s="5" t="s">
         <v>695</v>
-      </c>
-      <c r="C184" s="5" t="s">
-        <v>696</v>
       </c>
       <c r="E184" t="str">
         <f t="shared" si="5"/>
@@ -6130,10 +6139,10 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
+        <v>646</v>
+      </c>
+      <c r="B186" s="5" t="s">
         <v>647</v>
-      </c>
-      <c r="B186" s="5" t="s">
-        <v>648</v>
       </c>
       <c r="C186" s="5" t="s">
         <v>292</v>
@@ -6237,10 +6246,10 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
+        <v>648</v>
+      </c>
+      <c r="B193" s="5" t="s">
         <v>649</v>
-      </c>
-      <c r="B193" s="5" t="s">
-        <v>650</v>
       </c>
       <c r="C193" s="5" t="s">
         <v>300</v>
@@ -6252,10 +6261,10 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
+        <v>632</v>
+      </c>
+      <c r="B194" s="5" t="s">
         <v>633</v>
-      </c>
-      <c r="B194" s="5" t="s">
-        <v>634</v>
       </c>
       <c r="C194" s="5" t="s">
         <v>292</v>
@@ -6267,10 +6276,10 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
+        <v>625</v>
+      </c>
+      <c r="B195" s="5" t="s">
         <v>626</v>
-      </c>
-      <c r="B195" s="5" t="s">
-        <v>627</v>
       </c>
       <c r="C195" s="5" t="s">
         <v>182</v>
@@ -6426,10 +6435,10 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
+        <v>634</v>
+      </c>
+      <c r="B205" s="5" t="s">
         <v>635</v>
-      </c>
-      <c r="B205" s="5" t="s">
-        <v>636</v>
       </c>
       <c r="C205" s="5" t="s">
         <v>292</v>
@@ -6519,10 +6528,10 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="B211" s="5" t="s">
         <v>669</v>
-      </c>
-      <c r="B211" s="5" t="s">
-        <v>670</v>
       </c>
       <c r="C211" s="5" t="s">
         <v>300</v>
@@ -6631,10 +6640,10 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B218" s="5" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C218" s="5" t="s">
         <v>442</v>
@@ -6707,10 +6716,10 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="B223" s="5" t="s">
         <v>660</v>
-      </c>
-      <c r="B223" s="5" t="s">
-        <v>661</v>
       </c>
       <c r="C223" s="5" t="s">
         <v>292</v>
@@ -6752,10 +6761,10 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
+        <v>670</v>
+      </c>
+      <c r="B226" s="5" t="s">
         <v>671</v>
-      </c>
-      <c r="B226" s="5" t="s">
-        <v>672</v>
       </c>
       <c r="C226" s="5" t="s">
         <v>300</v>
@@ -6840,10 +6849,10 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="B232" s="5" t="s">
         <v>713</v>
-      </c>
-      <c r="B232" s="5" t="s">
-        <v>714</v>
       </c>
       <c r="C232" s="5" t="s">
         <v>292</v>
@@ -6960,10 +6969,10 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="B240" s="5" t="s">
         <v>683</v>
-      </c>
-      <c r="B240" s="5" t="s">
-        <v>684</v>
       </c>
       <c r="C240" s="5" t="s">
         <v>292</v>
@@ -7020,10 +7029,10 @@
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="B244" s="5" t="s">
         <v>656</v>
-      </c>
-      <c r="B244" s="5" t="s">
-        <v>657</v>
       </c>
       <c r="C244" s="5" t="s">
         <v>292</v>
@@ -7051,10 +7060,10 @@
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="5" t="s">
+        <v>661</v>
+      </c>
+      <c r="B246" s="5" t="s">
         <v>662</v>
-      </c>
-      <c r="B246" s="5" t="s">
-        <v>663</v>
       </c>
       <c r="C246" s="5" t="s">
         <v>292</v>
@@ -7158,10 +7167,10 @@
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="5" t="s">
+        <v>657</v>
+      </c>
+      <c r="B253" s="5" t="s">
         <v>658</v>
-      </c>
-      <c r="B253" s="5" t="s">
-        <v>659</v>
       </c>
       <c r="C253" s="5" t="s">
         <v>292</v>
@@ -7173,10 +7182,10 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="5" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C254" s="5" t="s">
         <v>292</v>
@@ -7188,10 +7197,10 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="5" t="s">
+        <v>742</v>
+      </c>
+      <c r="B255" s="5" t="s">
         <v>743</v>
-      </c>
-      <c r="B255" s="5" t="s">
-        <v>744</v>
       </c>
       <c r="C255" s="5" t="s">
         <v>300</v>
@@ -7203,10 +7212,10 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="5" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="C256" s="5" t="s">
         <v>300</v>
@@ -7264,10 +7273,10 @@
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="B260" s="5" t="s">
         <v>609</v>
-      </c>
-      <c r="B260" s="5" t="s">
-        <v>610</v>
       </c>
       <c r="C260" s="5" t="s">
         <v>292</v>
@@ -7279,10 +7288,10 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="5" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B261" s="5" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C261" s="5" t="s">
         <v>442</v>
@@ -7324,10 +7333,10 @@
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="5" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="B264" s="5" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="C264" s="5" t="s">
         <v>300</v>
@@ -7354,10 +7363,10 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="B266" s="5" t="s">
         <v>605</v>
-      </c>
-      <c r="B266" s="5" t="s">
-        <v>606</v>
       </c>
       <c r="C266" s="5" t="s">
         <v>300</v>
@@ -7414,16 +7423,16 @@
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="5" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B270" s="5" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C270" s="5" t="s">
         <v>292</v>
       </c>
       <c r="D270" s="5" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E270" t="str">
         <f t="shared" si="8"/>
@@ -7432,10 +7441,10 @@
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="B271" s="5" t="s">
         <v>708</v>
-      </c>
-      <c r="B271" s="5" t="s">
-        <v>709</v>
       </c>
       <c r="C271" s="5" t="s">
         <v>300</v>
@@ -7462,10 +7471,10 @@
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="5" t="s">
+        <v>672</v>
+      </c>
+      <c r="B273" s="5" t="s">
         <v>673</v>
-      </c>
-      <c r="B273" s="5" t="s">
-        <v>674</v>
       </c>
       <c r="C273" s="5" t="s">
         <v>424</v>
@@ -7477,10 +7486,10 @@
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="B274" s="5" t="s">
         <v>719</v>
-      </c>
-      <c r="B274" s="5" t="s">
-        <v>720</v>
       </c>
       <c r="C274" s="5" t="s">
         <v>300</v>
@@ -7577,7 +7586,7 @@
         <v>292</v>
       </c>
       <c r="D280" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E280">
         <f t="shared" si="8"/>
@@ -7632,10 +7641,10 @@
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="B284" s="5" t="s">
         <v>737</v>
-      </c>
-      <c r="B284" s="5" t="s">
-        <v>738</v>
       </c>
       <c r="C284" s="5" t="s">
         <v>300</v>
@@ -7647,10 +7656,10 @@
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="5" t="s">
+        <v>734</v>
+      </c>
+      <c r="B285" s="5" t="s">
         <v>735</v>
-      </c>
-      <c r="B285" s="5" t="s">
-        <v>736</v>
       </c>
       <c r="C285" s="5" t="s">
         <v>292</v>
@@ -7693,7 +7702,7 @@
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="5" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B288" s="5" t="s">
         <v>434</v>
@@ -7817,10 +7826,10 @@
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="B296" s="5" t="s">
         <v>727</v>
-      </c>
-      <c r="B296" s="5" t="s">
-        <v>728</v>
       </c>
       <c r="C296" s="5" t="s">
         <v>300</v>
@@ -7939,10 +7948,10 @@
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="B304" s="5" t="s">
         <v>725</v>
-      </c>
-      <c r="B304" s="5" t="s">
-        <v>726</v>
       </c>
       <c r="C304" s="5" t="s">
         <v>424</v>
@@ -8031,10 +8040,10 @@
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="5" t="s">
+        <v>666</v>
+      </c>
+      <c r="B310" s="5" t="s">
         <v>667</v>
-      </c>
-      <c r="B310" s="5" t="s">
-        <v>668</v>
       </c>
       <c r="C310" s="5" t="s">
         <v>292</v>
@@ -8061,7 +8070,7 @@
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B312" s="5" t="s">
         <v>489</v>
@@ -8079,7 +8088,7 @@
         <v>488</v>
       </c>
       <c r="B313" s="5" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C313" s="5" t="s">
         <v>292</v>
@@ -8107,10 +8116,10 @@
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="5" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B315" s="5" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C315" s="5" t="s">
         <v>300</v>
@@ -8448,10 +8457,10 @@
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="5" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B337" s="5" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C337" s="5" t="s">
         <v>300</v>
@@ -8463,10 +8472,10 @@
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="B338" s="5" t="s">
         <v>702</v>
-      </c>
-      <c r="B338" s="5" t="s">
-        <v>703</v>
       </c>
       <c r="C338" s="5" t="s">
         <v>300</v>
@@ -8494,10 +8503,10 @@
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="B340" s="5" t="s">
         <v>680</v>
-      </c>
-      <c r="B340" s="5" t="s">
-        <v>681</v>
       </c>
       <c r="C340" s="5" t="s">
         <v>292</v>
@@ -8524,10 +8533,10 @@
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="5" t="s">
+        <v>627</v>
+      </c>
+      <c r="B342" s="5" t="s">
         <v>628</v>
-      </c>
-      <c r="B342" s="5" t="s">
-        <v>629</v>
       </c>
       <c r="C342" s="5" t="s">
         <v>292</v>
@@ -8615,10 +8624,10 @@
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="B348" s="5" t="s">
         <v>723</v>
-      </c>
-      <c r="B348" s="5" t="s">
-        <v>724</v>
       </c>
       <c r="C348" s="5" t="s">
         <v>292</v>
@@ -8630,10 +8639,10 @@
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="B349" s="5" t="s">
         <v>699</v>
-      </c>
-      <c r="B349" s="5" t="s">
-        <v>700</v>
       </c>
       <c r="C349" s="5" t="s">
         <v>300</v>
@@ -8661,10 +8670,10 @@
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B351" s="5" t="s">
-        <v>751</v>
+        <v>809</v>
       </c>
       <c r="C351" s="5" t="s">
         <v>292</v>
@@ -8676,10 +8685,10 @@
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="B352" s="5" t="s">
         <v>731</v>
-      </c>
-      <c r="B352" s="5" t="s">
-        <v>732</v>
       </c>
       <c r="C352" s="5" t="s">
         <v>292</v>
@@ -8737,10 +8746,10 @@
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="B356" s="5" t="s">
         <v>654</v>
-      </c>
-      <c r="B356" s="5" t="s">
-        <v>655</v>
       </c>
       <c r="C356" s="5" t="s">
         <v>292</v>
@@ -8767,10 +8776,10 @@
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="5" t="s">
+        <v>644</v>
+      </c>
+      <c r="B358" s="5" t="s">
         <v>645</v>
-      </c>
-      <c r="B358" s="5" t="s">
-        <v>646</v>
       </c>
       <c r="C358" s="5" t="s">
         <v>292</v>
@@ -8782,10 +8791,10 @@
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="B359" s="5" t="s">
         <v>607</v>
-      </c>
-      <c r="B359" s="5" t="s">
-        <v>608</v>
       </c>
       <c r="C359" s="5" t="s">
         <v>292</v>
@@ -8813,10 +8822,10 @@
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="5" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="B361" s="5" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C361" s="5" t="s">
         <v>442</v>
@@ -8846,10 +8855,10 @@
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="5" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B363" s="5" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C363" s="5" t="s">
         <v>292</v>
@@ -8861,10 +8870,10 @@
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="5" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B364" s="5" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C364" s="5" t="s">
         <v>292</v>
@@ -9079,10 +9088,10 @@
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="5" t="s">
+        <v>738</v>
+      </c>
+      <c r="B378" s="5" t="s">
         <v>739</v>
-      </c>
-      <c r="B378" s="5" t="s">
-        <v>740</v>
       </c>
       <c r="C378" s="5" t="s">
         <v>424</v>
@@ -9198,10 +9207,10 @@
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A385" s="5" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B385" s="5" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C385" s="5" t="s">
         <v>292</v>
@@ -9213,10 +9222,10 @@
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A386" s="5" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B386" s="5" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="C386" s="5" t="s">
         <v>292</v>
@@ -9228,10 +9237,10 @@
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A387" s="5" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="B387" s="5" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C387" s="5" t="s">
         <v>292</v>
@@ -9243,10 +9252,10 @@
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A388" s="5" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B388" s="5" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C388" s="5" t="s">
         <v>292</v>
@@ -9258,16 +9267,16 @@
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A389" s="5" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="B389" s="5" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="C389" s="5" t="s">
         <v>300</v>
       </c>
       <c r="D389" s="5" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="E389" t="str">
         <f t="shared" si="10"/>
@@ -9276,10 +9285,10 @@
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A390" s="5" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B390" s="5" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C390" s="5" t="s">
         <v>595</v>
@@ -9291,10 +9300,10 @@
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A391" s="5" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B391" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C391" s="5" t="s">
         <v>300</v>
@@ -9306,10 +9315,10 @@
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A392" s="5" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B392" s="5" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="C392" s="5" t="s">
         <v>292</v>
@@ -9321,10 +9330,10 @@
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A393" s="5" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B393" s="5" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="C393" s="5" t="s">
         <v>300</v>
@@ -9336,10 +9345,10 @@
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A394" s="5" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B394" s="5" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="C394" s="5" t="s">
         <v>300</v>
@@ -9351,10 +9360,10 @@
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A395" s="5" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B395" s="5" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="C395" s="5" t="s">
         <v>300</v>
@@ -9365,9 +9374,14 @@
       </c>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B396" s="5"/>
+      <c r="A396" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="B396" s="5" t="s">
+        <v>806</v>
+      </c>
       <c r="C396" s="5" t="s">
-        <v>156</v>
+        <v>300</v>
       </c>
       <c r="E396" t="str">
         <f t="shared" si="10"/>
@@ -9375,9 +9389,14 @@
       </c>
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B397" s="5"/>
+      <c r="A397" s="5" t="s">
+        <v>807</v>
+      </c>
+      <c r="B397" s="5" t="s">
+        <v>808</v>
+      </c>
       <c r="C397" s="5" t="s">
-        <v>156</v>
+        <v>424</v>
       </c>
       <c r="E397" t="str">
         <f t="shared" si="10"/>
@@ -15391,7 +15410,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" x14ac:dyDescent="0.25">
@@ -15409,7 +15428,7 @@
     </row>
     <row r="5" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
@@ -15419,12 +15438,12 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
@@ -15434,12 +15453,12 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
SFRmaker #7: pre-pixi update
</commit_message>
<xml_diff>
--- a/Mng/Acronyms.xlsx
+++ b/Mng/Acronyms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OD\WS_Mdl\Mng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8783954C-362C-485F-AD84-8545388E6839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36894D1-ACE6-4A5E-B768-4B9E972EE9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -307,7 +307,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1831" uniqueCount="813">
   <si>
     <t>GW</t>
   </si>
@@ -2741,6 +2741,12 @@
   </si>
   <si>
     <t>Elevation</t>
+  </si>
+  <si>
+    <t>Sgm</t>
+  </si>
+  <si>
+    <t>Segment</t>
   </si>
 </sst>
 </file>
@@ -3279,8 +3285,8 @@
   <dimension ref="A1:F994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D81" sqref="D81"/>
+      <pane ySplit="1" topLeftCell="A369" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D398" sqref="D398"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9407,9 +9413,14 @@
       </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B398" s="5"/>
+      <c r="A398" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="B398" s="5" t="s">
+        <v>812</v>
+      </c>
       <c r="C398" s="5" t="s">
-        <v>156</v>
+        <v>300</v>
       </c>
       <c r="E398" t="str">
         <f t="shared" si="10"/>

</xml_diff>

<commit_message>
SFRmaker #11: NBr34 succeeded!
Need to get CHDs till 2020 from Deltares, then I can let it run over the weekend. I can continue with the SFRmaker debugging for now.
</commit_message>
<xml_diff>
--- a/Mng/Acronyms.xlsx
+++ b/Mng/Acronyms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OD\WS_Mdl\Mng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36894D1-ACE6-4A5E-B768-4B9E972EE9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0F4A7C-05F2-45F0-8B6B-B4C6B5AFF450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3285,8 +3285,8 @@
   <dimension ref="A1:F994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A369" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D398" sqref="D398"/>
+      <pane ySplit="1" topLeftCell="A363" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D395" sqref="D395"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
SFRmaker #12: NBr34 ready to be run. p_TS_range.py created.
</commit_message>
<xml_diff>
--- a/Mng/Acronyms.xlsx
+++ b/Mng/Acronyms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OD\WS_Mdl\Mng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0F4A7C-05F2-45F0-8B6B-B4C6B5AFF450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1F36EB-E075-4F95-951D-05DF1784935C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acronyms" sheetId="1" r:id="rId1"/>
@@ -307,7 +307,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1831" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="815">
   <si>
     <t>GW</t>
   </si>
@@ -2747,6 +2747,12 @@
   </si>
   <si>
     <t>Segment</t>
+  </si>
+  <si>
+    <t>p_</t>
+  </si>
+  <si>
+    <t>plot</t>
   </si>
 </sst>
 </file>
@@ -3285,8 +3291,8 @@
   <dimension ref="A1:F994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A363" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D395" sqref="D395"/>
+      <pane ySplit="1" topLeftCell="A364" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A400" sqref="A400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9428,9 +9434,14 @@
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B399" s="5"/>
+      <c r="A399" s="5" t="s">
+        <v>813</v>
+      </c>
+      <c r="B399" s="5" t="s">
+        <v>814</v>
+      </c>
       <c r="C399" s="5" t="s">
-        <v>156</v>
+        <v>424</v>
       </c>
       <c r="E399" t="str">
         <f t="shared" si="10"/>

</xml_diff>

<commit_message>
SFRmaker #14: NBr34 'finished'. NBr33 more debugging
geo.py: Added decimals option to DA_to_MBTIF
utils.py: Added paths. Improved formatting. Addd DF_info.
setup.py: o_VS added.
NBr34.smk: Improvements.
</commit_message>
<xml_diff>
--- a/Mng/Acronyms.xlsx
+++ b/Mng/Acronyms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OD\WS_Mdl\Mng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1F36EB-E075-4F95-951D-05DF1784935C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47276DC3-A639-496B-A914-5CEDC18A199A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acronyms" sheetId="1" r:id="rId1"/>
@@ -307,7 +307,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="817">
   <si>
     <t>GW</t>
   </si>
@@ -1438,9 +1438,6 @@
     <t>Wcs</t>
   </si>
   <si>
-    <t>Bae-Flow</t>
-  </si>
-  <si>
     <t>Available/Availability</t>
   </si>
   <si>
@@ -1714,9 +1711,6 @@
     <t>Interaction</t>
   </si>
   <si>
-    <t>Inf</t>
-  </si>
-  <si>
     <t>Inflow</t>
   </si>
   <si>
@@ -2753,6 +2747,18 @@
   </si>
   <si>
     <t>plot</t>
+  </si>
+  <si>
+    <t>Base-Flow</t>
+  </si>
+  <si>
+    <t>InFl</t>
+  </si>
+  <si>
+    <t>OuFl</t>
+  </si>
+  <si>
+    <t>Out-Flow</t>
   </si>
 </sst>
 </file>
@@ -3291,8 +3297,8 @@
   <dimension ref="A1:F994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A364" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A400" sqref="A400"/>
+      <pane ySplit="1" topLeftCell="A366" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C401" sqref="C401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3315,7 +3321,7 @@
         <v>155</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>81</v>
@@ -3345,10 +3351,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>292</v>
@@ -3360,13 +3366,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -3375,13 +3381,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -3406,10 +3412,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>386</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>387</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>300</v>
@@ -3421,10 +3427,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>388</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>389</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>300</v>
@@ -3436,10 +3442,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>390</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>391</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>300</v>
@@ -3534,10 +3540,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>290</v>
@@ -3549,10 +3555,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>406</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>407</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>290</v>
@@ -3579,7 +3585,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>58</v>
@@ -3595,10 +3601,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>452</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>453</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>300</v>
@@ -3610,10 +3616,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>415</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>416</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>300</v>
@@ -3625,16 +3631,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>300</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
@@ -3662,7 +3668,7 @@
         <v>224</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>300</v>
@@ -3674,7 +3680,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>51</v>
@@ -3693,7 +3699,7 @@
         <v>356</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>376</v>
+        <v>813</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>290</v>
@@ -3721,10 +3727,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>292</v>
@@ -3751,10 +3757,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>292</v>
@@ -3766,10 +3772,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>300</v>
@@ -3797,13 +3803,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
@@ -3812,10 +3818,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>300</v>
@@ -3827,13 +3833,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" ref="E34:E65" si="1">IF(AND(A34=A33,A34&lt;&gt;""),1,"")</f>
@@ -3842,10 +3848,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>418</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>419</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>300</v>
@@ -3872,7 +3878,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>69</v>
@@ -3888,10 +3894,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>292</v>
@@ -3903,10 +3909,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>300</v>
@@ -3918,10 +3924,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>292</v>
@@ -3933,10 +3939,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>300</v>
@@ -3948,10 +3954,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>292</v>
@@ -3963,10 +3969,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>300</v>
@@ -3978,10 +3984,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>300</v>
@@ -3993,10 +3999,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>463</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>464</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>292</v>
@@ -4008,10 +4014,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>292</v>
@@ -4042,10 +4048,10 @@
         <v>275</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E48">
         <f t="shared" si="1"/>
@@ -4057,7 +4063,7 @@
         <v>275</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>293</v>
@@ -4105,10 +4111,10 @@
         <v>260</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E52">
         <f t="shared" si="1"/>
@@ -4117,10 +4123,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>292</v>
@@ -4132,10 +4138,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>300</v>
@@ -4162,13 +4168,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>432</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>433</v>
-      </c>
       <c r="C56" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="1"/>
@@ -4177,10 +4183,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>454</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>455</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>182</v>
@@ -4208,10 +4214,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>300</v>
@@ -4238,13 +4244,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>444</v>
-      </c>
       <c r="C61" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="1"/>
@@ -4268,13 +4274,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E63">
         <f t="shared" si="1"/>
@@ -4283,13 +4289,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E64" t="str">
         <f t="shared" si="1"/>
@@ -4298,13 +4304,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E65" t="str">
         <f t="shared" si="1"/>
@@ -4313,10 +4319,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>292</v>
@@ -4373,13 +4379,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E70">
         <f t="shared" si="2"/>
@@ -4403,10 +4409,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>292</v>
@@ -4418,10 +4424,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>292</v>
@@ -4433,10 +4439,10 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>300</v>
@@ -4590,10 +4596,10 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>292</v>
@@ -4635,10 +4641,10 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>300</v>
@@ -4666,10 +4672,10 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>300</v>
@@ -4681,10 +4687,10 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="B90" s="5" t="s">
         <v>396</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>397</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>300</v>
@@ -4696,10 +4702,10 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B91" s="5" t="s">
         <v>394</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>395</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>300</v>
@@ -4711,10 +4717,10 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>300</v>
@@ -4726,13 +4732,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E93">
         <f t="shared" si="2"/>
@@ -4741,10 +4747,10 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>292</v>
@@ -4802,10 +4808,10 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>292</v>
@@ -4817,10 +4823,10 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>292</v>
@@ -4832,10 +4838,10 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>292</v>
@@ -4862,10 +4868,10 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>300</v>
@@ -4877,10 +4883,10 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>290</v>
@@ -4892,10 +4898,10 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>300</v>
@@ -4907,10 +4913,10 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>300</v>
@@ -4922,10 +4928,10 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="B106" s="5" t="s">
         <v>435</v>
-      </c>
-      <c r="B106" s="5" t="s">
-        <v>436</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>292</v>
@@ -4937,13 +4943,13 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="B107" s="5" t="s">
         <v>440</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="C107" s="5" t="s">
         <v>441</v>
-      </c>
-      <c r="C107" s="5" t="s">
-        <v>442</v>
       </c>
       <c r="E107" t="str">
         <f t="shared" si="3"/>
@@ -5015,10 +5021,10 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>292</v>
@@ -5030,10 +5036,10 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C113" s="5" t="s">
         <v>292</v>
@@ -5045,13 +5051,13 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E114" t="str">
         <f t="shared" si="3"/>
@@ -5125,13 +5131,13 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="11" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E119" t="str">
         <f t="shared" si="3"/>
@@ -5155,10 +5161,10 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C121" s="5" t="s">
         <v>300</v>
@@ -5232,10 +5238,10 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="B126" s="5" t="s">
         <v>380</v>
-      </c>
-      <c r="B126" s="5" t="s">
-        <v>381</v>
       </c>
       <c r="C126" s="5" t="s">
         <v>290</v>
@@ -5247,10 +5253,10 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="B127" s="5" t="s">
         <v>409</v>
-      </c>
-      <c r="B127" s="5" t="s">
-        <v>410</v>
       </c>
       <c r="C127" s="5" t="s">
         <v>290</v>
@@ -5277,10 +5283,10 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C129" s="5" t="s">
         <v>292</v>
@@ -5369,10 +5375,10 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="B135" s="5" t="s">
         <v>392</v>
-      </c>
-      <c r="B135" s="5" t="s">
-        <v>393</v>
       </c>
       <c r="C135" s="5" t="s">
         <v>290</v>
@@ -5399,10 +5405,10 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="B137" s="5" t="s">
         <v>461</v>
-      </c>
-      <c r="B137" s="5" t="s">
-        <v>462</v>
       </c>
       <c r="C137" s="5" t="s">
         <v>292</v>
@@ -5432,7 +5438,7 @@
         <v>311</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C139" s="5" t="s">
         <v>292</v>
@@ -5474,10 +5480,10 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C142" s="5" t="s">
         <v>292</v>
@@ -5489,10 +5495,10 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C143" s="5" t="s">
         <v>300</v>
@@ -5519,13 +5525,13 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="11" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B145" s="11" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E145" t="str">
         <f t="shared" si="4"/>
@@ -5534,10 +5540,10 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C146" s="5" t="s">
         <v>300</v>
@@ -5579,13 +5585,13 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="11" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B149" s="11" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E149" t="str">
         <f t="shared" si="4"/>
@@ -5594,16 +5600,16 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E150" t="str">
         <f t="shared" si="4"/>
@@ -5642,10 +5648,10 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>468</v>
+        <v>814</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C153" s="5" t="s">
         <v>292</v>
@@ -5657,10 +5663,10 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="C154" s="5" t="s">
         <v>300</v>
@@ -5672,13 +5678,13 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="B155" s="5" t="s">
         <v>430</v>
       </c>
-      <c r="B155" s="5" t="s">
-        <v>431</v>
-      </c>
       <c r="C155" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E155" t="str">
         <f t="shared" si="4"/>
@@ -5687,10 +5693,10 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C156" s="5" t="s">
         <v>300</v>
@@ -5702,10 +5708,10 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C157" s="5" t="s">
         <v>300</v>
@@ -5732,10 +5738,10 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C159" s="5" t="s">
         <v>292</v>
@@ -5743,10 +5749,10 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="C160" s="5" t="s">
         <v>300</v>
@@ -5758,10 +5764,10 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C161" s="5" t="s">
         <v>292</v>
@@ -5834,7 +5840,7 @@
         <v>296</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="E165" t="str">
         <f t="shared" si="5"/>
@@ -5843,13 +5849,13 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="B166" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="B166" s="5" t="s">
+      <c r="C166" s="5" t="s">
         <v>423</v>
-      </c>
-      <c r="C166" s="5" t="s">
-        <v>424</v>
       </c>
       <c r="E166">
         <f t="shared" si="5"/>
@@ -5861,7 +5867,7 @@
         <v>294</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="C167" s="5" t="s">
         <v>292</v>
@@ -5873,13 +5879,13 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="11" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B168" s="11" t="s">
         <v>173</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E168" t="str">
         <f t="shared" si="5"/>
@@ -5888,10 +5894,10 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C169" s="5" t="s">
         <v>292</v>
@@ -5903,10 +5909,10 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C170" s="5" t="s">
         <v>300</v>
@@ -5933,13 +5939,13 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="11" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B172" s="11" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E172" t="str">
         <f t="shared" si="5"/>
@@ -5981,10 +5987,10 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C175" s="5" t="s">
         <v>292</v>
@@ -6094,13 +6100,13 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="11" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B182" s="11" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E182" t="str">
         <f t="shared" si="5"/>
@@ -6109,10 +6115,10 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="B183" s="5" t="s">
         <v>456</v>
-      </c>
-      <c r="B183" s="5" t="s">
-        <v>457</v>
       </c>
       <c r="C183" s="5" t="s">
         <v>182</v>
@@ -6124,13 +6130,13 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
+        <v>691</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="C184" s="5" t="s">
         <v>693</v>
-      </c>
-      <c r="B184" s="5" t="s">
-        <v>694</v>
-      </c>
-      <c r="C184" s="5" t="s">
-        <v>695</v>
       </c>
       <c r="E184" t="str">
         <f t="shared" si="5"/>
@@ -6154,10 +6160,10 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C186" s="5" t="s">
         <v>292</v>
@@ -6169,10 +6175,10 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="B187" s="5" t="s">
         <v>413</v>
-      </c>
-      <c r="B187" s="5" t="s">
-        <v>414</v>
       </c>
       <c r="C187" s="5" t="s">
         <v>290</v>
@@ -6199,10 +6205,10 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="B189" s="5" t="s">
         <v>458</v>
-      </c>
-      <c r="B189" s="5" t="s">
-        <v>459</v>
       </c>
       <c r="C189" s="5" t="s">
         <v>182</v>
@@ -6214,10 +6220,10 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C190" s="5" t="s">
         <v>292</v>
@@ -6261,10 +6267,10 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C193" s="5" t="s">
         <v>300</v>
@@ -6276,10 +6282,10 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B194" s="5" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C194" s="5" t="s">
         <v>292</v>
@@ -6291,10 +6297,10 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B195" s="5" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C195" s="5" t="s">
         <v>182</v>
@@ -6306,13 +6312,13 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="11" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B196" s="11" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E196" t="str">
         <f t="shared" si="6"/>
@@ -6358,7 +6364,7 @@
         <v>3</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C199" s="5" t="s">
         <v>292</v>
@@ -6435,10 +6441,10 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C204" s="5" t="s">
         <v>300</v>
@@ -6450,10 +6456,10 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B205" s="5" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C205" s="5" t="s">
         <v>292</v>
@@ -6543,10 +6549,10 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B211" s="5" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C211" s="5" t="s">
         <v>300</v>
@@ -6590,13 +6596,13 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="11" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B214" s="11" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C214" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E214" t="str">
         <f t="shared" si="6"/>
@@ -6655,13 +6661,13 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B218" s="5" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C218" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E218" t="str">
         <f t="shared" si="6"/>
@@ -6701,13 +6707,13 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="11" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B221" s="11" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C221" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E221" t="str">
         <f t="shared" si="6"/>
@@ -6716,10 +6722,10 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C222" s="5" t="s">
         <v>292</v>
@@ -6731,10 +6737,10 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C223" s="5" t="s">
         <v>292</v>
@@ -6746,10 +6752,10 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="B224" s="5" t="s">
         <v>411</v>
-      </c>
-      <c r="B224" s="5" t="s">
-        <v>412</v>
       </c>
       <c r="C224" s="5" t="s">
         <v>300</v>
@@ -6776,10 +6782,10 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C226" s="5" t="s">
         <v>300</v>
@@ -6806,13 +6812,13 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="5" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C228" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E228" t="str">
         <f t="shared" si="6"/>
@@ -6864,10 +6870,10 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C232" s="5" t="s">
         <v>292</v>
@@ -6879,7 +6885,7 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="5" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B233" s="5" t="s">
         <v>299</v>
@@ -6894,10 +6900,10 @@
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="B234" s="5" t="s">
         <v>437</v>
-      </c>
-      <c r="B234" s="5" t="s">
-        <v>438</v>
       </c>
       <c r="C234" s="5" t="s">
         <v>292</v>
@@ -6909,10 +6915,10 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C235" s="5" t="s">
         <v>290</v>
@@ -6924,10 +6930,10 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C236" s="5" t="s">
         <v>290</v>
@@ -6984,10 +6990,10 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="5" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B240" s="5" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="C240" s="5" t="s">
         <v>292</v>
@@ -7029,10 +7035,10 @@
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="5" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B243" s="5" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C243" s="5" t="s">
         <v>292</v>
@@ -7044,10 +7050,10 @@
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="5" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B244" s="5" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C244" s="5" t="s">
         <v>292</v>
@@ -7075,10 +7081,10 @@
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="5" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C246" s="5" t="s">
         <v>292</v>
@@ -7090,7 +7096,7 @@
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="6" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B247" s="5" t="s">
         <v>31</v>
@@ -7106,10 +7112,10 @@
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="11" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B248" s="12" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C248" s="5" t="s">
         <v>292</v>
@@ -7136,10 +7142,10 @@
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="5" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C250" s="5" t="s">
         <v>300</v>
@@ -7167,10 +7173,10 @@
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="5" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B252" s="5" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C252" s="5" t="s">
         <v>292</v>
@@ -7182,10 +7188,10 @@
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="5" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B253" s="5" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C253" s="5" t="s">
         <v>292</v>
@@ -7197,10 +7203,10 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="5" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C254" s="5" t="s">
         <v>292</v>
@@ -7212,10 +7218,10 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="5" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C255" s="5" t="s">
         <v>300</v>
@@ -7227,10 +7233,10 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="5" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="C256" s="5" t="s">
         <v>300</v>
@@ -7288,10 +7294,10 @@
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="5" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B260" s="5" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C260" s="5" t="s">
         <v>292</v>
@@ -7303,13 +7309,13 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="5" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="B261" s="5" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C261" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E261" t="str">
         <f t="shared" si="8"/>
@@ -7318,10 +7324,10 @@
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="B262" s="5" t="s">
         <v>378</v>
-      </c>
-      <c r="B262" s="5" t="s">
-        <v>379</v>
       </c>
       <c r="C262" s="5" t="s">
         <v>290</v>
@@ -7333,13 +7339,13 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="11" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B263" s="11" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C263" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E263">
         <f t="shared" si="8"/>
@@ -7348,10 +7354,10 @@
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="5" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B264" s="5" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="C264" s="5" t="s">
         <v>300</v>
@@ -7378,10 +7384,10 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="5" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B266" s="5" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C266" s="5" t="s">
         <v>300</v>
@@ -7393,10 +7399,10 @@
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B267" s="5" t="s">
         <v>445</v>
-      </c>
-      <c r="B267" s="5" t="s">
-        <v>446</v>
       </c>
       <c r="C267" s="5" t="s">
         <v>300</v>
@@ -7408,10 +7414,10 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B268" s="5" t="s">
         <v>384</v>
-      </c>
-      <c r="B268" s="5" t="s">
-        <v>385</v>
       </c>
       <c r="C268" s="5" t="s">
         <v>300</v>
@@ -7423,10 +7429,10 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="B269" s="5" t="s">
         <v>398</v>
-      </c>
-      <c r="B269" s="5" t="s">
-        <v>399</v>
       </c>
       <c r="C269" s="5" t="s">
         <v>290</v>
@@ -7438,16 +7444,16 @@
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="5" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="B270" s="5" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="C270" s="5" t="s">
         <v>292</v>
       </c>
       <c r="D270" s="5" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E270" t="str">
         <f t="shared" si="8"/>
@@ -7456,10 +7462,10 @@
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="5" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B271" s="5" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C271" s="5" t="s">
         <v>300</v>
@@ -7471,13 +7477,13 @@
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="11" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B272" s="11" t="s">
         <v>172</v>
       </c>
       <c r="C272" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E272" t="str">
         <f t="shared" si="8"/>
@@ -7486,13 +7492,13 @@
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="5" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B273" s="5" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C273" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E273" t="str">
         <f t="shared" si="8"/>
@@ -7501,10 +7507,10 @@
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="5" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B274" s="5" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="C274" s="5" t="s">
         <v>300</v>
@@ -7531,10 +7537,10 @@
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B276" s="5" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C276" s="5" t="s">
         <v>292</v>
@@ -7577,13 +7583,13 @@
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="B279" s="5" t="s">
         <v>426</v>
       </c>
-      <c r="B279" s="5" t="s">
-        <v>427</v>
-      </c>
       <c r="C279" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E279">
         <f t="shared" si="8"/>
@@ -7601,7 +7607,7 @@
         <v>292</v>
       </c>
       <c r="D280" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E280">
         <f t="shared" si="8"/>
@@ -7610,10 +7616,10 @@
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="5" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B281" s="5" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C281" s="5" t="s">
         <v>292</v>
@@ -7656,10 +7662,10 @@
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="5" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="C284" s="5" t="s">
         <v>300</v>
@@ -7671,10 +7677,10 @@
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="5" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C285" s="5" t="s">
         <v>292</v>
@@ -7717,13 +7723,13 @@
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="5" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B288" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C288" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D288" s="5"/>
       <c r="E288" t="str">
@@ -7781,13 +7787,13 @@
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="11" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B292" s="11" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C292" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E292" t="str">
         <f t="shared" si="8"/>
@@ -7796,13 +7802,13 @@
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="11" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B293" s="11" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C293" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E293" t="str">
         <f t="shared" si="8"/>
@@ -7811,10 +7817,10 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B294" s="5" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C294" s="5" t="s">
         <v>292</v>
@@ -7841,10 +7847,10 @@
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="5" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B296" s="5" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="C296" s="5" t="s">
         <v>300</v>
@@ -7872,10 +7878,10 @@
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="5" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B298" s="5" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C298" s="5" t="s">
         <v>292</v>
@@ -7887,10 +7893,10 @@
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="5" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B299" s="5" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C299" s="5" t="s">
         <v>292</v>
@@ -7933,10 +7939,10 @@
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="5" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B302" s="5" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C302" s="5" t="s">
         <v>292</v>
@@ -7948,10 +7954,10 @@
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="5" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B303" s="5" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C303" s="5" t="s">
         <v>292</v>
@@ -7963,13 +7969,13 @@
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="5" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B304" s="5" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="C304" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E304" t="str">
         <f t="shared" si="8"/>
@@ -7994,13 +8000,13 @@
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="11" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B306" s="11" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C306" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E306" t="str">
         <f t="shared" si="8"/>
@@ -8040,10 +8046,10 @@
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="5" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B309" s="5" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C309" s="5" t="s">
         <v>292</v>
@@ -8055,10 +8061,10 @@
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="5" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B310" s="5" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C310" s="5" t="s">
         <v>292</v>
@@ -8070,10 +8076,10 @@
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="5" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B311" s="5" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C311" s="5" t="s">
         <v>292</v>
@@ -8085,10 +8091,10 @@
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="5" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="B312" s="5" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C312" s="5" t="s">
         <v>292</v>
@@ -8100,10 +8106,10 @@
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="5" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B313" s="5" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="C313" s="5" t="s">
         <v>292</v>
@@ -8131,10 +8137,10 @@
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="5" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B315" s="5" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C315" s="5" t="s">
         <v>300</v>
@@ -8146,10 +8152,10 @@
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="B316" s="5" t="s">
         <v>447</v>
-      </c>
-      <c r="B316" s="5" t="s">
-        <v>448</v>
       </c>
       <c r="C316" s="5" t="s">
         <v>300</v>
@@ -8177,10 +8183,10 @@
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B318" s="5" t="s">
         <v>420</v>
-      </c>
-      <c r="B318" s="5" t="s">
-        <v>421</v>
       </c>
       <c r="C318" s="5" t="s">
         <v>292</v>
@@ -8192,10 +8198,10 @@
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="5" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B319" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C319" s="5" t="s">
         <v>292</v>
@@ -8223,13 +8229,13 @@
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="11" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B321" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C321" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E321">
         <f t="shared" si="9"/>
@@ -8253,10 +8259,10 @@
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="B323" s="5" t="s">
         <v>382</v>
-      </c>
-      <c r="B323" s="5" t="s">
-        <v>383</v>
       </c>
       <c r="C323" s="5" t="s">
         <v>290</v>
@@ -8427,13 +8433,13 @@
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="B334" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="B334" s="5" t="s">
-        <v>429</v>
-      </c>
       <c r="C334" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E334">
         <f t="shared" si="9"/>
@@ -8442,13 +8448,13 @@
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="11" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B335" s="11" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C335" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E335" t="str">
         <f t="shared" si="9"/>
@@ -8472,10 +8478,10 @@
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="5" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B337" s="5" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="C337" s="5" t="s">
         <v>300</v>
@@ -8487,10 +8493,10 @@
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="5" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B338" s="5" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C338" s="5" t="s">
         <v>300</v>
@@ -8518,10 +8524,10 @@
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="5" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B340" s="5" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C340" s="5" t="s">
         <v>292</v>
@@ -8548,10 +8554,10 @@
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="5" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B342" s="5" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C342" s="5" t="s">
         <v>292</v>
@@ -8594,10 +8600,10 @@
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="5" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B345" s="5" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C345" s="5" t="s">
         <v>292</v>
@@ -8609,10 +8615,10 @@
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="5" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B346" s="5" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C346" s="5" t="s">
         <v>156</v>
@@ -8624,10 +8630,10 @@
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="B347" s="5" t="s">
         <v>449</v>
-      </c>
-      <c r="B347" s="5" t="s">
-        <v>450</v>
       </c>
       <c r="C347" s="5" t="s">
         <v>300</v>
@@ -8639,10 +8645,10 @@
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="5" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="B348" s="5" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C348" s="5" t="s">
         <v>292</v>
@@ -8654,10 +8660,10 @@
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="5" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B349" s="5" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C349" s="5" t="s">
         <v>300</v>
@@ -8685,10 +8691,10 @@
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="5" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B351" s="5" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="C351" s="5" t="s">
         <v>292</v>
@@ -8700,10 +8706,10 @@
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="5" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B352" s="5" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C352" s="5" t="s">
         <v>292</v>
@@ -8731,13 +8737,13 @@
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="11" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B354" s="11" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C354" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E354" t="str">
         <f t="shared" si="9"/>
@@ -8746,13 +8752,13 @@
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="11" t="s">
+        <v>591</v>
+      </c>
+      <c r="B355" s="11" t="s">
+        <v>592</v>
+      </c>
+      <c r="C355" s="5" t="s">
         <v>593</v>
-      </c>
-      <c r="B355" s="11" t="s">
-        <v>594</v>
-      </c>
-      <c r="C355" s="5" t="s">
-        <v>595</v>
       </c>
       <c r="E355" t="str">
         <f t="shared" si="9"/>
@@ -8761,10 +8767,10 @@
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="5" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B356" s="5" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C356" s="5" t="s">
         <v>292</v>
@@ -8791,10 +8797,10 @@
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="5" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B358" s="5" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C358" s="5" t="s">
         <v>292</v>
@@ -8806,10 +8812,10 @@
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="5" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B359" s="5" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C359" s="5" t="s">
         <v>292</v>
@@ -8837,13 +8843,13 @@
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="5" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="B361" s="5" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="C361" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E361" t="str">
         <f t="shared" si="9"/>
@@ -8870,10 +8876,10 @@
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="5" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B363" s="5" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="C363" s="5" t="s">
         <v>292</v>
@@ -8885,10 +8891,10 @@
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="5" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B364" s="5" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C364" s="5" t="s">
         <v>292</v>
@@ -8903,7 +8909,7 @@
         <v>375</v>
       </c>
       <c r="B365" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C365" s="5" t="s">
         <v>290</v>
@@ -8946,13 +8952,13 @@
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="11" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B368" s="11" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C368" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E368" t="str">
         <f t="shared" si="9"/>
@@ -8976,10 +8982,10 @@
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="5" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B370" s="5" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C370" s="5" t="s">
         <v>292</v>
@@ -9042,7 +9048,7 @@
         <v>32</v>
       </c>
       <c r="B374" s="5" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C374" s="5" t="s">
         <v>290</v>
@@ -9054,7 +9060,7 @@
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="6" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B375" s="5" t="s">
         <v>33</v>
@@ -9103,13 +9109,13 @@
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="5" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B378" s="5" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C378" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E378" t="str">
         <f t="shared" si="10"/>
@@ -9222,10 +9228,10 @@
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A385" s="5" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="B385" s="5" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C385" s="5" t="s">
         <v>292</v>
@@ -9237,10 +9243,10 @@
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A386" s="5" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B386" s="5" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C386" s="5" t="s">
         <v>292</v>
@@ -9252,10 +9258,10 @@
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A387" s="5" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B387" s="5" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="C387" s="5" t="s">
         <v>292</v>
@@ -9267,10 +9273,10 @@
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A388" s="5" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="B388" s="5" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C388" s="5" t="s">
         <v>292</v>
@@ -9282,16 +9288,16 @@
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A389" s="5" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B389" s="5" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C389" s="5" t="s">
         <v>300</v>
       </c>
       <c r="D389" s="5" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E389" t="str">
         <f t="shared" si="10"/>
@@ -9300,13 +9306,13 @@
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A390" s="5" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B390" s="5" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C390" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E390" t="str">
         <f t="shared" si="10"/>
@@ -9315,10 +9321,10 @@
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A391" s="5" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B391" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C391" s="5" t="s">
         <v>300</v>
@@ -9330,10 +9336,10 @@
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A392" s="5" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B392" s="5" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C392" s="5" t="s">
         <v>292</v>
@@ -9345,10 +9351,10 @@
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A393" s="5" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B393" s="5" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="C393" s="5" t="s">
         <v>300</v>
@@ -9360,10 +9366,10 @@
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A394" s="5" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B394" s="5" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="C394" s="5" t="s">
         <v>300</v>
@@ -9375,10 +9381,10 @@
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A395" s="5" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B395" s="5" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="C395" s="5" t="s">
         <v>300</v>
@@ -9390,10 +9396,10 @@
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A396" s="5" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B396" s="5" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="C396" s="5" t="s">
         <v>300</v>
@@ -9405,13 +9411,13 @@
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A397" s="5" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B397" s="5" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="C397" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E397" t="str">
         <f t="shared" si="10"/>
@@ -9420,10 +9426,10 @@
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A398" s="5" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B398" s="5" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="C398" s="5" t="s">
         <v>300</v>
@@ -9435,13 +9441,13 @@
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A399" s="5" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B399" s="5" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="C399" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E399" t="str">
         <f t="shared" si="10"/>
@@ -9449,9 +9455,14 @@
       </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B400" s="5"/>
+      <c r="A400" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="B400" s="5" t="s">
+        <v>816</v>
+      </c>
       <c r="C400" s="5" t="s">
-        <v>156</v>
+        <v>300</v>
       </c>
       <c r="E400" t="str">
         <f t="shared" si="10"/>
@@ -15435,7 +15446,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" x14ac:dyDescent="0.25">
@@ -15443,7 +15454,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.25">
@@ -15453,22 +15464,22 @@
     </row>
     <row r="5" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
@@ -15478,17 +15489,17 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
SFRmaker #15: NBr34 re-run. NBr35 runs incorrectly.
It seems that there are no outlets in NBr35. I'll investigate that, then re-run it.
</commit_message>
<xml_diff>
--- a/Mng/Acronyms.xlsx
+++ b/Mng/Acronyms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OD\WS_Mdl\Mng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47276DC3-A639-496B-A914-5CEDC18A199A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B969736-7105-437E-A6B5-72710D4CD5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acronyms" sheetId="1" r:id="rId1"/>
@@ -307,7 +307,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1835" uniqueCount="817">
   <si>
     <t>GW</t>
   </si>
@@ -3297,8 +3297,8 @@
   <dimension ref="A1:F994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A366" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C401" sqref="C401"/>
+      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B163" sqref="B163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
SFRmaker #16: NBr35 corrections. geo.SFR_to_GPkg improvemetns.
NBr35 had errors in it's Cfg files (BAT, PRJ), fixed them so that the Sim starts at 1993, like NBr34.
geo.SFR_to_GPk only worked with specifix col names. Made it more versatile. It now creates an outlfow point file and a routing file.
</commit_message>
<xml_diff>
--- a/Mng/Acronyms.xlsx
+++ b/Mng/Acronyms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OD\WS_Mdl\Mng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B969736-7105-437E-A6B5-72710D4CD5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54B34BC-4C20-45AD-9A12-65939B46A87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acronyms" sheetId="1" r:id="rId1"/>
@@ -3297,8 +3297,8 @@
   <dimension ref="A1:F994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B163" sqref="B163"/>
+      <pane ySplit="1" topLeftCell="A359" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A377" sqref="A377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
forgot to 'git add .'...
</commit_message>
<xml_diff>
--- a/Mng/Acronyms.xlsx
+++ b/Mng/Acronyms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BF88D8-C04D-4914-8956-2AB4A1F1637D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9954B7A-324B-4E40-AAB1-096D4103129D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -307,7 +307,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="842">
   <si>
     <t>GW</t>
   </si>
@@ -2828,6 +2828,12 @@
   </si>
   <si>
     <t>iBridges</t>
+  </si>
+  <si>
+    <t>Rmt</t>
+  </si>
+  <si>
+    <t>Remote</t>
   </si>
 </sst>
 </file>
@@ -9719,9 +9725,14 @@
       </c>
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B413" s="5"/>
+      <c r="A413" s="5" t="s">
+        <v>840</v>
+      </c>
+      <c r="B413" s="5" t="s">
+        <v>841</v>
+      </c>
       <c r="C413" s="5" t="s">
-        <v>156</v>
+        <v>292</v>
       </c>
       <c r="E413" t="str">
         <f t="shared" si="12"/>

</xml_diff>